<commit_message>
Update new alias types for label_structure.xlsx
</commit_message>
<xml_diff>
--- a/Classification of information requests from Members/label_structure/label_structure.xlsx
+++ b/Classification of information requests from Members/label_structure/label_structure.xlsx
@@ -1,31 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JiaHui\鴻海\新幹班\test_ncuproj_classification\Classification of information requests from Members\label_structure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victor/Documents/Labs/Ayla/test_ncuproj_classification/Classification of information requests from Members/label_structure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA505995-6FC5-4FD1-81E4-E3A00F58CD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{42318CB5-52CE-4DA7-A55B-EA7D7EEA3B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26130" yWindow="2670" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29460" yWindow="4740" windowWidth="26880" windowHeight="19160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="一二級機關" sheetId="1" r:id="rId1"/>
+    <sheet name="別名對應" sheetId="2" r:id="rId2"/>
+    <sheet name="要保留二級的局處" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="130">
   <si>
     <t>primary</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,6 +71,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>區公所</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>財政局</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -71,26 +88,30 @@
     <t>教育局</t>
   </si>
   <si>
+    <t>圖書館</t>
+  </si>
+  <si>
+    <t>動物園</t>
+  </si>
+  <si>
+    <t>教師研習中心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>天文科學教育館</t>
   </si>
   <si>
     <t>臺北市家庭教育中心</t>
   </si>
   <si>
-    <t>教師研習中心</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>圖書館</t>
-  </si>
-  <si>
-    <t>動物園</t>
-  </si>
-  <si>
     <t>市立大學</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>高級中學</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>高級職業學校</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -115,15 +136,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>市場處</t>
+  </si>
+  <si>
     <t>商業處</t>
   </si>
   <si>
     <t>動物保護處</t>
   </si>
   <si>
-    <t>市場處</t>
-  </si>
-  <si>
     <t>工務局</t>
   </si>
   <si>
@@ -143,11 +164,15 @@
   </si>
   <si>
     <t>交通局</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>停車管理工程處</t>
   </si>
   <si>
+    <t>交通局</t>
+  </si>
+  <si>
     <t>交通管制工程處</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -158,10 +183,6 @@
     <t>交通事件裁決所</t>
   </si>
   <si>
-    <t>交通局</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>社會局</t>
   </si>
   <si>
@@ -284,6 +305,16 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>第一區工程處</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二區工程處</t>
+  </si>
+  <si>
+    <t>機電系統工程處</t>
+  </si>
+  <si>
     <t>臺北翡翠水庫管理局</t>
   </si>
   <si>
@@ -322,16 +353,16 @@
     <t>主計處</t>
   </si>
   <si>
+    <t>人事處</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>政風處</t>
   </si>
   <si>
     <t>公務人員訓練處</t>
   </si>
   <si>
-    <t>人事處</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>研究發展考核委員會</t>
   </si>
   <si>
@@ -354,21 +385,98 @@
     <t>臺北大眾捷運股份有限公司</t>
   </si>
   <si>
-    <t>區公所</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高級中學</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第二區工程處</t>
-  </si>
-  <si>
-    <t>機電系統工程處</t>
-  </si>
-  <si>
-    <t>第一區工程處</t>
+    <t>簡稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>對應名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教研中心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>研考會</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>研究發展考核委員會</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客委會</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客家事務委員會</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>觀傳局</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>觀光傳播局</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原民會</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原住民族事務委員會</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>產業局</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>青少年發展暨家庭教育中心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>臺北市家庭教育中心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>臺北市青少年發展暨家庭教育中心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刑警大隊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>環保局</t>
+  </si>
+  <si>
+    <t>環境保護局</t>
+  </si>
+  <si>
+    <t>捷運局</t>
+  </si>
+  <si>
+    <t>捷運工程局</t>
+  </si>
+  <si>
+    <t>都發局</t>
+  </si>
+  <si>
+    <t>都市發展局</t>
+  </si>
+  <si>
+    <t>北水處</t>
+  </si>
+  <si>
+    <t>臺北自來水事業處</t>
+  </si>
+  <si>
+    <t>捷運公司</t>
+  </si>
+  <si>
+    <t>工務局</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -398,12 +506,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -418,9 +532,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -703,14 +818,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1"/>
   <cols>
-    <col min="1" max="1" width="29.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -753,129 +869,129 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15">
+    <row r="6" spans="1:2" ht="17.100000000000001">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>99</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
@@ -883,458 +999,637 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B54" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B56" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B59" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B63" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B64" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B65" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B67" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B68" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B69" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B83" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>98</v>
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF424271-18F1-9A41-A66F-247CE21451CD}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.1"/>
+  <cols>
+    <col min="1" max="1" width="41.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="14.25">
+      <c r="A14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4300F110-A3EB-DB4D-965C-FF00A26F34C7}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.1"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>